<commit_message>
Updated pinouts, added all information
</commit_message>
<xml_diff>
--- a/pinouts.xlsx
+++ b/pinouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Top Left</t>
   </si>
@@ -33,6 +33,54 @@
   </si>
   <si>
     <t>Wifi Switch</t>
+  </si>
+  <si>
+    <t>Left Light</t>
+  </si>
+  <si>
+    <t>Resistor on Right</t>
+  </si>
+  <si>
+    <t>Middle Light</t>
+  </si>
+  <si>
+    <t>Right Light</t>
+  </si>
+  <si>
+    <t>Push Button</t>
+  </si>
+  <si>
+    <t>Motion Sensor Ground</t>
+  </si>
+  <si>
+    <t>Motion Sensor 3.3V</t>
+  </si>
+  <si>
+    <t>Motion Sensor Data</t>
+  </si>
+  <si>
+    <t>Light Sensor</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>Motion Sensor</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Common Items</t>
+  </si>
+  <si>
+    <t>Note the left and right are swapped by the ribbon cable, with reference to the pinout.</t>
+  </si>
+  <si>
+    <t>Top is defined as the side AWAY from the USB</t>
+  </si>
+  <si>
+    <t>Left is defined as the side with the HDMI</t>
   </si>
 </sst>
 </file>
@@ -48,12 +96,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF85E5E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,14 +146,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF33CCCC"/>
+      <color rgb="FFF85E5E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -384,55 +476,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" s="5">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -440,47 +578,77 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="C7">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>13</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>15</v>
       </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="C9">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C10">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>19</v>
       </c>
       <c r="C11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>21</v>
       </c>
@@ -488,7 +656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23</v>
       </c>
@@ -496,15 +664,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>25</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C14">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>27</v>
       </c>
@@ -512,15 +689,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>29</v>
       </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C16">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>31</v>
       </c>
@@ -528,7 +714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>33</v>
       </c>
@@ -536,7 +722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>35</v>
       </c>
@@ -544,25 +730,34 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>37</v>
       </c>
+      <c r="B20" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="C20">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>39</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C21">
         <v>40</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added backup motion sensor button
</commit_message>
<xml_diff>
--- a/pinouts.xlsx
+++ b/pinouts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Wifi Switch</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>192.168.42.139</t>
+  </si>
+  <si>
+    <t>Backup Motion Sensor Button</t>
+  </si>
+  <si>
+    <t>Backup Motion Sensor Button Gnd</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,8 +693,20 @@
       <c r="A7">
         <v>9</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D7">
         <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1">
+        <v>16</v>
       </c>
       <c r="I7" t="s">
         <v>27</v>

</xml_diff>